<commit_message>
removed in correct sku split logic
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VisheshPhutela\Projects\Forecasting tool\simu_expo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CBDDC2E-88F7-478F-A0A0-55F37722076C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9862B10E-F3E2-46BB-934D-41494B81DD9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3320" uniqueCount="651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3322" uniqueCount="653">
   <si>
     <t>Forecast Name</t>
   </si>
@@ -1987,18 +1988,25 @@
   </si>
   <si>
     <t>$94,50,02,625</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Forecast</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="#,##0%"/>
     <numFmt numFmtId="165" formatCode="[$-14009]yyyy/mm/dd;@"/>
     <numFmt numFmtId="166" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="167" formatCode="&quot;₹&quot;\ #,##0.00"/>
+    <numFmt numFmtId="168" formatCode="mmm/yyyy"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -2056,7 +2064,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2081,6 +2089,11 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -11591,7 +11604,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{943FF1DB-F012-4FB5-96C3-73700FE7C401}">
   <dimension ref="A1:GW274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
@@ -20604,4 +20617,350 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7138666-3AE0-4312-959C-FCE96E8FBE29}">
+  <dimension ref="A1:B37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>651</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="13">
+        <v>46023</v>
+      </c>
+      <c r="B2" s="14">
+        <v>6360</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <f>EDATE(A2,1)</f>
+        <v>46054</v>
+      </c>
+      <c r="B3" s="14">
+        <v>17280</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <f>EDATE(A3,1)</f>
+        <v>46082</v>
+      </c>
+      <c r="B4" s="14">
+        <v>17820</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <f>EDATE(A4,1)</f>
+        <v>46113</v>
+      </c>
+      <c r="B5" s="14">
+        <v>24240</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <f>EDATE(A5,1)</f>
+        <v>46143</v>
+      </c>
+      <c r="B6" s="14">
+        <v>33060</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <f>EDATE(A6,1)</f>
+        <v>46174</v>
+      </c>
+      <c r="B7" s="14">
+        <v>28680</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <f>EDATE(A7,1)</f>
+        <v>46204</v>
+      </c>
+      <c r="B8" s="14">
+        <v>31980</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
+        <f>EDATE(A8,1)</f>
+        <v>46235</v>
+      </c>
+      <c r="B9" s="14">
+        <v>40500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <f>EDATE(A9,1)</f>
+        <v>46266</v>
+      </c>
+      <c r="B10" s="14">
+        <v>34620</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
+        <f>EDATE(A10,1)</f>
+        <v>46296</v>
+      </c>
+      <c r="B11" s="14">
+        <v>37740</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="13">
+        <f>EDATE(A11,1)</f>
+        <v>46327</v>
+      </c>
+      <c r="B12" s="14">
+        <v>48900</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="13">
+        <f>EDATE(A12,1)</f>
+        <v>46357</v>
+      </c>
+      <c r="B13" s="14">
+        <v>40080</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
+        <f>EDATE(A13,1)</f>
+        <v>46388</v>
+      </c>
+      <c r="B14" s="14">
+        <v>43080</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="13">
+        <f>EDATE(A14,1)</f>
+        <v>46419</v>
+      </c>
+      <c r="B15" s="14">
+        <v>60420</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="13">
+        <f>EDATE(A15,1)</f>
+        <v>46447</v>
+      </c>
+      <c r="B16" s="14">
+        <v>51420</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="13">
+        <f>EDATE(A16,1)</f>
+        <v>46478</v>
+      </c>
+      <c r="B17" s="14">
+        <v>56820</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="13">
+        <f>EDATE(A17,1)</f>
+        <v>46508</v>
+      </c>
+      <c r="B18" s="14">
+        <v>76320</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="13">
+        <f>EDATE(A18,1)</f>
+        <v>46539</v>
+      </c>
+      <c r="B19" s="14">
+        <v>68820</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="13">
+        <f>EDATE(A19,1)</f>
+        <v>46569</v>
+      </c>
+      <c r="B20" s="14">
+        <v>74220</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="13">
+        <f>EDATE(A20,1)</f>
+        <v>46600</v>
+      </c>
+      <c r="B21" s="14">
+        <v>91440</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="13">
+        <f>EDATE(A21,1)</f>
+        <v>46631</v>
+      </c>
+      <c r="B22" s="14">
+        <v>72900</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="13">
+        <f>EDATE(A22,1)</f>
+        <v>46661</v>
+      </c>
+      <c r="B23" s="14">
+        <v>80880</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="13">
+        <f>EDATE(A23,1)</f>
+        <v>46692</v>
+      </c>
+      <c r="B24" s="14">
+        <v>99840</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="13">
+        <f>EDATE(A24,1)</f>
+        <v>46722</v>
+      </c>
+      <c r="B25" s="14">
+        <v>86280</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="13">
+        <f>EDATE(A25,1)</f>
+        <v>46753</v>
+      </c>
+      <c r="B26" s="14">
+        <v>88860</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="13">
+        <f>EDATE(A26,1)</f>
+        <v>46784</v>
+      </c>
+      <c r="B27" s="14">
+        <v>126960</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="13">
+        <f>EDATE(A27,1)</f>
+        <v>46813</v>
+      </c>
+      <c r="B28" s="14">
+        <v>98760</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="13">
+        <f>EDATE(A28,1)</f>
+        <v>46844</v>
+      </c>
+      <c r="B29" s="14">
+        <v>100080</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="13">
+        <f>EDATE(A29,1)</f>
+        <v>46874</v>
+      </c>
+      <c r="B30" s="14">
+        <v>125040</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="13">
+        <f>EDATE(A30,1)</f>
+        <v>46905</v>
+      </c>
+      <c r="B31" s="14">
+        <v>109320</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="13">
+        <f>EDATE(A31,1)</f>
+        <v>46935</v>
+      </c>
+      <c r="B32" s="14">
+        <v>117060</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="13">
+        <f>EDATE(A32,1)</f>
+        <v>46966</v>
+      </c>
+      <c r="B33" s="14">
+        <v>155160</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="13">
+        <f>EDATE(A33,1)</f>
+        <v>46997</v>
+      </c>
+      <c r="B34" s="14">
+        <v>147600</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="13">
+        <f>EDATE(A34,1)</f>
+        <v>47027</v>
+      </c>
+      <c r="B35" s="14">
+        <v>144900</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="13">
+        <f>EDATE(A35,1)</f>
+        <v>47058</v>
+      </c>
+      <c r="B36" s="14">
+        <v>173460</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="13">
+        <f>EDATE(A36,1)</f>
+        <v>47088</v>
+      </c>
+      <c r="B37" s="14">
+        <v>152580</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>